<commit_message>
Index sections made collapsable. Bootstrap references uodated. Videogame (hangedman) back-end and front-end code finished
</commit_message>
<xml_diff>
--- a/1Homework/DataBase/Heart.xlsx
+++ b/1Homework/DataBase/Heart.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R9a8c98f7c44744a3"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R04e6c87cfccf42cf"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -36,8 +36,8 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFF0000"/>
-        <x:bgColor rgb="FFFF0000"/>
+        <x:fgColor rgb="FFF00000"/>
+        <x:bgColor rgb="FFF00000"/>
       </x:patternFill>
     </x:fill>
   </x:fills>

</xml_diff>